<commit_message>
tous les nosej integer et noseqsej en had
</commit_message>
<xml_diff>
--- a/formats/excel/Formats RAPSS 11.xlsx
+++ b/formats/excel/Formats RAPSS 11.xlsx
@@ -1,370 +1,700 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27815"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumepressiat/Documents/R/pmeasyr_versions/pmeasyr_0.2/formats/excel/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="460" windowWidth="27340" windowHeight="17540"/>
+    <workbookView windowWidth="24240" windowHeight="12855"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104">
+  <si>
+    <t>nom</t>
+  </si>
+  <si>
+    <t>longueur</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>fin</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>verif</t>
+  </si>
+  <si>
+    <t>libelle</t>
+  </si>
+  <si>
+    <t>NOFINESS</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
   <si>
     <t>Numéro FINESS de l’entité juridique</t>
   </si>
   <si>
+    <t>NOVRAPSS</t>
+  </si>
+  <si>
     <t>Numéro de version du format de RAPSS</t>
   </si>
   <si>
+    <t>NOFINESS_GEO</t>
+  </si>
+  <si>
+    <t>Numéro FINESS de l’établissement (code géographique)</t>
+  </si>
+  <si>
+    <t>NOSEQSEJ</t>
+  </si>
+  <si>
     <t>Numéro séquentiel de séjour d'HAD</t>
   </si>
   <si>
+    <t>AGEAN</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
     <t>Âge en années</t>
   </si>
   <si>
+    <t>AGEJR</t>
+  </si>
+  <si>
     <t>Âge en jours</t>
   </si>
   <si>
+    <t>SEXE</t>
+  </si>
+  <si>
     <t>Sexe du patient</t>
   </si>
   <si>
+    <t>CDGEO</t>
+  </si>
+  <si>
     <t>Code géographique</t>
   </si>
   <si>
+    <t>TYPDOM</t>
+  </si>
+  <si>
     <t>Type de lieu de domicile du patient</t>
   </si>
   <si>
+    <t>NOFINESS_ESMS</t>
+  </si>
+  <si>
     <t>Numéro FINESS EHPA</t>
   </si>
   <si>
+    <t>DUREESEJ</t>
+  </si>
+  <si>
     <t>Nombre de journées dans le séjour</t>
   </si>
   <si>
+    <t>MODE_ENTREE</t>
+  </si>
+  <si>
     <t>Mode d’entrée</t>
   </si>
   <si>
+    <t>PROVENANCE</t>
+  </si>
+  <si>
     <t>Provenance</t>
   </si>
   <si>
+    <t>MODE_SORTIE</t>
+  </si>
+  <si>
     <t>Mode de sortie</t>
   </si>
   <si>
+    <t>DESTINATION</t>
+  </si>
+  <si>
     <t>Destination</t>
   </si>
   <si>
+    <t>MOISSOR_SEJ</t>
+  </si>
+  <si>
     <t>Mois de la date de sortie du séjour</t>
   </si>
   <si>
+    <t>ANSOR_SEJ</t>
+  </si>
+  <si>
     <t>Année de la date de sortie du séjour</t>
   </si>
   <si>
+    <t>NOSEQ</t>
+  </si>
+  <si>
     <t>Numéro de la séquence dans le séjour</t>
   </si>
   <si>
+    <t>NB_JR_DB_SEQ</t>
+  </si>
+  <si>
+    <t>Nombre de journées entre le début de la séquence et la date d’entrée du séjour</t>
+  </si>
+  <si>
+    <t>DUREE_SEQ</t>
+  </si>
+  <si>
     <t>Nombre de journées dans la séquence</t>
   </si>
   <si>
+    <t>DERNIERE_SEQ</t>
+  </si>
+  <si>
     <t>Dernière séquence</t>
   </si>
   <si>
+    <t>MOIS_FIN_SEQ</t>
+  </si>
+  <si>
     <t>Mois de la date de fin de la séquence</t>
   </si>
   <si>
+    <t>AN_FIN_SEQ</t>
+  </si>
+  <si>
     <t>Année de la date de fin de la séquence</t>
   </si>
   <si>
+    <t>MPP</t>
+  </si>
+  <si>
     <t>Mode de prise en charge principal</t>
   </si>
   <si>
+    <t>MPA</t>
+  </si>
+  <si>
     <t>Mode de prise en charge associé</t>
   </si>
   <si>
+    <t>MPCAD1</t>
+  </si>
+  <si>
+    <t>Mode de prise en charge associé documentaire 1</t>
+  </si>
+  <si>
+    <t>MPCAD2</t>
+  </si>
+  <si>
+    <t>Mode de prise en charge associé documentaire 2</t>
+  </si>
+  <si>
+    <t>MPCAD3</t>
+  </si>
+  <si>
+    <t>Mode de prise en charge associé documentaire 3</t>
+  </si>
+  <si>
+    <t>MPCAD4</t>
+  </si>
+  <si>
+    <t>Mode de prise en charge associé documentaire 4</t>
+  </si>
+  <si>
+    <t>MPCAD5</t>
+  </si>
+  <si>
+    <t>Mode de prise en charge associé documentaire 5</t>
+  </si>
+  <si>
+    <t>IK</t>
+  </si>
+  <si>
     <t>Cotation dépendance selon Karnofsky</t>
   </si>
   <si>
+    <t>DP</t>
+  </si>
+  <si>
     <t>Diagnostic principal</t>
   </si>
   <si>
+    <t>NBDA</t>
+  </si>
+  <si>
     <t>Nombre de diagnostics associés (NbDa)</t>
   </si>
   <si>
+    <t>HABILLAGE</t>
+  </si>
+  <si>
     <t xml:space="preserve"> habillage/toilette</t>
   </si>
   <si>
+    <t>LOCOMOT</t>
+  </si>
+  <si>
     <t xml:space="preserve"> locomotion</t>
   </si>
   <si>
+    <t>ALIMENT</t>
+  </si>
+  <si>
     <t xml:space="preserve"> alimentation</t>
   </si>
   <si>
+    <t>CONTINENCE</t>
+  </si>
+  <si>
     <t xml:space="preserve"> continence</t>
   </si>
   <si>
+    <t>COMPORTEMENT</t>
+  </si>
+  <si>
     <t xml:space="preserve"> comportement</t>
   </si>
   <si>
+    <t>RELATION</t>
+  </si>
+  <si>
     <t xml:space="preserve"> relation</t>
   </si>
   <si>
+    <t>NOSOUSSEQ</t>
+  </si>
+  <si>
     <t>Numéro de sousséquence</t>
   </si>
   <si>
+    <t>MOIS_FIN_SS_SEQ</t>
+  </si>
+  <si>
     <t>Mois de sortie de la sousséquence</t>
   </si>
   <si>
+    <t>AN_FIN_SS_SEQ</t>
+  </si>
+  <si>
     <t>Année de sortie de la sousséquence</t>
   </si>
   <si>
+    <t>NB_JR_DB_SS_SEQ</t>
+  </si>
+  <si>
+    <t>Nombre de journées entre le début de la sousséquence et le début de la séquence</t>
+  </si>
+  <si>
+    <t>DUREE_SS_SEQ</t>
+  </si>
+  <si>
     <t>Nombre de journées de la sousséquence</t>
   </si>
   <si>
+    <t>DER_SS_SEQ</t>
+  </si>
+  <si>
     <t>Dernière sousséquence de la séquence</t>
   </si>
   <si>
+    <t>DER_SS_SEQ_SEJ</t>
+  </si>
+  <si>
     <t>Dernière sousséquence du séjour</t>
   </si>
   <si>
+    <t>NBZA</t>
+  </si>
+  <si>
     <t>Nombre de zones d'actes CCAM (NbZa)</t>
   </si>
   <si>
-    <t>Numéro FINESS de l’établissement (code géographique)</t>
-  </si>
-  <si>
-    <t>Mode de prise en charge associé documentaire 1</t>
-  </si>
-  <si>
-    <t>Mode de prise en charge associé documentaire 2</t>
-  </si>
-  <si>
-    <t>Mode de prise en charge associé documentaire 3</t>
-  </si>
-  <si>
-    <t>Mode de prise en charge associé documentaire 4</t>
-  </si>
-  <si>
-    <t>Mode de prise en charge associé documentaire 5</t>
-  </si>
-  <si>
-    <t>Nombre de journées entre le début de la séquence et la date d’entrée du séjour</t>
-  </si>
-  <si>
-    <t>Nombre de journées entre le début de la sousséquence et le début de la séquence</t>
-  </si>
-  <si>
     <t>Z</t>
-  </si>
-  <si>
-    <t>libelle</t>
-  </si>
-  <si>
-    <t>verif</t>
-  </si>
-  <si>
-    <t>position</t>
-  </si>
-  <si>
-    <t>longueur</t>
-  </si>
-  <si>
-    <t>fin</t>
-  </si>
-  <si>
-    <t>nom</t>
-  </si>
-  <si>
-    <t>NOFINESS</t>
-  </si>
-  <si>
-    <t>NOVRAPSS</t>
-  </si>
-  <si>
-    <t>NOFINESS_GEO</t>
-  </si>
-  <si>
-    <t>NOSEJHAD</t>
-  </si>
-  <si>
-    <t>AGEAN</t>
-  </si>
-  <si>
-    <t>AGEJR</t>
-  </si>
-  <si>
-    <t>SEXE</t>
-  </si>
-  <si>
-    <t>CDGEO</t>
-  </si>
-  <si>
-    <t>TYPDOM</t>
-  </si>
-  <si>
-    <t>NOFINESS_ESMS</t>
-  </si>
-  <si>
-    <t>DUREESEJ</t>
-  </si>
-  <si>
-    <t>MODE_ENTREE</t>
-  </si>
-  <si>
-    <t>PROVENANCE</t>
-  </si>
-  <si>
-    <t>MODE_SORTIE</t>
-  </si>
-  <si>
-    <t>DESTINATION</t>
-  </si>
-  <si>
-    <t>MOISSOR_SEJ</t>
-  </si>
-  <si>
-    <t>ANSOR_SEJ</t>
-  </si>
-  <si>
-    <t>NOSEQ</t>
-  </si>
-  <si>
-    <t>NB_JR_DB_SEQ</t>
-  </si>
-  <si>
-    <t>DUREE_SEQ</t>
-  </si>
-  <si>
-    <t>DERNIERE_SEQ</t>
-  </si>
-  <si>
-    <t>MOIS_FIN_SEQ</t>
-  </si>
-  <si>
-    <t>AN_FIN_SEQ</t>
-  </si>
-  <si>
-    <t>MPP</t>
-  </si>
-  <si>
-    <t>MPA</t>
-  </si>
-  <si>
-    <t>MPCAD1</t>
-  </si>
-  <si>
-    <t>MPCAD2</t>
-  </si>
-  <si>
-    <t>MPCAD3</t>
-  </si>
-  <si>
-    <t>MPCAD4</t>
-  </si>
-  <si>
-    <t>MPCAD5</t>
-  </si>
-  <si>
-    <t>IK</t>
-  </si>
-  <si>
-    <t>NBDA</t>
-  </si>
-  <si>
-    <t>HABILLAGE</t>
-  </si>
-  <si>
-    <t>LOCOMOT</t>
-  </si>
-  <si>
-    <t>ALIMENT</t>
-  </si>
-  <si>
-    <t>CONTINENCE</t>
-  </si>
-  <si>
-    <t>COMPORTEMENT</t>
-  </si>
-  <si>
-    <t>RELATION</t>
-  </si>
-  <si>
-    <t>NOSOUSSEQ</t>
-  </si>
-  <si>
-    <t>MOIS_FIN_SS_SEQ</t>
-  </si>
-  <si>
-    <t>AN_FIN_SS_SEQ</t>
-  </si>
-  <si>
-    <t>NB_JR_DB_SS_SEQ</t>
-  </si>
-  <si>
-    <t>DUREE_SS_SEQ</t>
-  </si>
-  <si>
-    <t>DER_SS_SEQ</t>
-  </si>
-  <si>
-    <t>DER_SS_SEQ_SEJ</t>
-  </si>
-  <si>
-    <t>NBZA</t>
-  </si>
-  <si>
-    <t>DP</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>i</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -372,23 +702,307 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
+    <cellStyle name="Comma[0]" xfId="20" builtinId="6"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Currency[0]" xfId="37" builtinId="7"/>
+    <cellStyle name="Heading 1" xfId="38" builtinId="16"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
+    <cellStyle name="Title" xfId="40" builtinId="15"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="20% - Accent1" xfId="42" builtinId="30"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="45" builtinId="17"/>
+    <cellStyle name="Comma" xfId="46" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="47" builtinId="23"/>
+    <cellStyle name="Percent" xfId="48" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -397,7 +1011,7 @@
   <a:themeElements>
     <a:clrScheme name="Bureau">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="4C4C4C"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -435,7 +1049,7 @@
     </a:clrScheme>
     <a:fontScheme name="Bureau">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -470,7 +1084,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -678,45 +1292,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="75.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="7" max="7" width="75.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>101</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>9</v>
@@ -728,19 +1343,19 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F2">
         <f>C2+B2-C3</f>
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -752,19 +1367,19 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F48" si="0">C3+B3-C4</f>
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>9</v>
@@ -776,19 +1391,19 @@
         <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -800,19 +1415,19 @@
         <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -824,19 +1439,19 @@
         <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>103</v>
+        <v>17</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -848,19 +1463,19 @@
         <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>103</v>
+        <v>17</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -872,19 +1487,19 @@
         <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="B9">
         <v>5</v>
@@ -896,19 +1511,19 @@
         <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -920,19 +1535,19 @@
         <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="B11">
         <v>9</v>
@@ -944,19 +1559,19 @@
         <v>48</v>
       </c>
       <c r="E11" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -968,19 +1583,19 @@
         <v>52</v>
       </c>
       <c r="E12" t="s">
-        <v>103</v>
+        <v>17</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -992,19 +1607,19 @@
         <v>53</v>
       </c>
       <c r="E13" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1016,19 +1631,19 @@
         <v>54</v>
       </c>
       <c r="E14" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1040,19 +1655,19 @@
         <v>55</v>
       </c>
       <c r="E15" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1064,19 +1679,19 @@
         <v>56</v>
       </c>
       <c r="E16" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -1088,19 +1703,19 @@
         <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -1112,19 +1727,19 @@
         <v>62</v>
       </c>
       <c r="E18" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -1136,19 +1751,19 @@
         <v>66</v>
       </c>
       <c r="E19" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -1160,19 +1775,19 @@
         <v>70</v>
       </c>
       <c r="E20" t="s">
-        <v>103</v>
+        <v>17</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -1184,19 +1799,19 @@
         <v>74</v>
       </c>
       <c r="E21" t="s">
-        <v>103</v>
+        <v>17</v>
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -1208,19 +1823,19 @@
         <v>75</v>
       </c>
       <c r="E22" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -1232,19 +1847,19 @@
         <v>77</v>
       </c>
       <c r="E23" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="B24">
         <v>4</v>
@@ -1256,19 +1871,19 @@
         <v>81</v>
       </c>
       <c r="E24" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -1280,19 +1895,19 @@
         <v>83</v>
       </c>
       <c r="E25" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -1304,19 +1919,19 @@
         <v>85</v>
       </c>
       <c r="E26" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -1328,19 +1943,19 @@
         <v>87</v>
       </c>
       <c r="E27" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -1352,19 +1967,19 @@
         <v>89</v>
       </c>
       <c r="E28" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -1376,19 +1991,19 @@
         <v>91</v>
       </c>
       <c r="E29" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -1400,19 +2015,19 @@
         <v>93</v>
       </c>
       <c r="E30" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -1424,19 +2039,19 @@
         <v>95</v>
       </c>
       <c r="E31" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -1448,19 +2063,19 @@
         <v>98</v>
       </c>
       <c r="E32" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G32" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="B33">
         <v>6</v>
@@ -1472,19 +2087,19 @@
         <v>104</v>
       </c>
       <c r="E33" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B34">
         <v>2</v>
@@ -1496,19 +2111,19 @@
         <v>106</v>
       </c>
       <c r="E34" t="s">
-        <v>103</v>
+        <v>17</v>
       </c>
       <c r="F34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G34" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -1520,19 +2135,19 @@
         <v>107</v>
       </c>
       <c r="E35" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G35" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -1544,19 +2159,19 @@
         <v>108</v>
       </c>
       <c r="E36" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G36" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -1568,19 +2183,19 @@
         <v>109</v>
       </c>
       <c r="E37" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F37">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -1592,19 +2207,19 @@
         <v>110</v>
       </c>
       <c r="E38" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -1616,19 +2231,19 @@
         <v>111</v>
       </c>
       <c r="E39" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F39">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G39" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -1640,19 +2255,19 @@
         <v>112</v>
       </c>
       <c r="E40" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G40" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B41">
         <v>4</v>
@@ -1664,19 +2279,19 @@
         <v>116</v>
       </c>
       <c r="E41" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F41">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G41" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B42">
         <v>2</v>
@@ -1688,19 +2303,19 @@
         <v>118</v>
       </c>
       <c r="E42" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F42">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G42" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B43">
         <v>4</v>
@@ -1712,19 +2327,19 @@
         <v>122</v>
       </c>
       <c r="E43" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G43" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B44">
         <v>4</v>
@@ -1736,19 +2351,19 @@
         <v>126</v>
       </c>
       <c r="E44" t="s">
-        <v>103</v>
+        <v>17</v>
       </c>
       <c r="F44">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G44" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B45">
         <v>4</v>
@@ -1760,17 +2375,17 @@
         <v>130</v>
       </c>
       <c r="E45" t="s">
-        <v>103</v>
+        <v>17</v>
       </c>
       <c r="F45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G45" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>97</v>
       </c>
@@ -1784,19 +2399,19 @@
         <v>131</v>
       </c>
       <c r="E46" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G46" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -1808,19 +2423,19 @@
         <v>132</v>
       </c>
       <c r="E47" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G47" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B48">
         <v>3</v>
@@ -1832,19 +2447,19 @@
         <v>135</v>
       </c>
       <c r="E48" t="s">
+        <v>17</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G48" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
         <v>103</v>
-      </c>
-      <c r="F48">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G48" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>47</v>
       </c>
       <c r="C49">
         <v>136</v>
@@ -1853,37 +2468,46 @@
         <v>145</v>
       </c>
       <c r="E49" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F49">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>